<commit_message>
kvalerio - download person template fixed
</commit_message>
<xml_diff>
--- a/public/files/xlsx/Plantilla_Invitados.xlsx
+++ b/public/files/xlsx/Plantilla_Invitados.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
+    <workbookView activeTab="1" autoFilterDateGrouping="true" firstSheet="0" minimized="false" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId4"/>
+    <sheet name="Personas" sheetId="1" r:id="rId4"/>
+    <sheet name="Subcategorias" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="1" fullCalcOnLoad="0" forceFullCalc="0"/>
@@ -20,27 +21,27 @@
     <t>Lista de personas</t>
   </si>
   <si>
+    <t>Cedula</t>
+  </si>
+  <si>
+    <t>Nombre</t>
+  </si>
+  <si>
+    <t>Apellido1</t>
+  </si>
+  <si>
+    <t>Apellido2</t>
+  </si>
+  <si>
+    <t>Correo</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
     <t>Subcategoria</t>
   </si>
   <si>
-    <t>Cedula</t>
-  </si>
-  <si>
-    <t>Nombre</t>
-  </si>
-  <si>
-    <t>Apellido1</t>
-  </si>
-  <si>
-    <t>Apellido2</t>
-  </si>
-  <si>
-    <t>Correo</t>
-  </si>
-  <si>
-    <t>Categoria</t>
-  </si>
-  <si>
     <t>Estado</t>
   </si>
   <si>
@@ -68,10 +69,16 @@
     <t>Estudiantes que reciben dinero y servicio de hospedaje</t>
   </si>
   <si>
-    <t>Emergencias</t>
-  </si>
-  <si>
-    <t>Equipos y más</t>
+    <t>Mario Soto</t>
+  </si>
+  <si>
+    <t>Emergencias y rescate</t>
+  </si>
+  <si>
+    <t>Equipos y mas</t>
+  </si>
+  <si>
+    <t>Karla Mora</t>
   </si>
   <si>
     <t>Mantenimientos</t>
@@ -80,22 +87,16 @@
     <t>Personal de limpieza de las areas de la universidads</t>
   </si>
   <si>
-    <t>Prueba</t>
-  </si>
-  <si>
-    <t>Desc Prueba</t>
-  </si>
-  <si>
-    <t>Prueba2</t>
-  </si>
-  <si>
-    <t>desc prueba2</t>
-  </si>
-  <si>
-    <t>Prueba 3</t>
-  </si>
-  <si>
-    <t>desc prueba 3 en vivo</t>
+    <t>Juan Vindas</t>
+  </si>
+  <si>
+    <t>Ingles B2</t>
+  </si>
+  <si>
+    <t>Equipo de grammar</t>
+  </si>
+  <si>
+    <t>Allicia Vega</t>
   </si>
 </sst>
 </file>
@@ -245,7 +246,7 @@
     <xf xfId="0" fontId="3" numFmtId="0" fillId="5" borderId="4" applyFont="1" applyNumberFormat="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="0" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0">
+    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
       <alignment textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>
@@ -547,13 +548,13 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q8"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A3" sqref="A3:XFD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="8.88671875" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="21.33203125" customWidth="true" style="0"/>
     <col min="2" max="2" width="23.6640625" customWidth="true" style="0"/>
@@ -585,33 +586,28 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
-      <c r="O1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="6"/>
     </row>
     <row r="2" spans="1:17" customHeight="1" ht="18">
       <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>8</v>
@@ -624,96 +620,126 @@
       </c>
       <c r="K2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="N3">
-        <v>18</v>
-      </c>
-      <c r="O3" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="N4">
-        <v>19</v>
-      </c>
-      <c r="O4" t="s">
-        <v>17</v>
-      </c>
-      <c r="P4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="N5">
-        <v>20</v>
-      </c>
-      <c r="O5" t="s">
-        <v>19</v>
-      </c>
-      <c r="P5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="N6">
-        <v>45</v>
-      </c>
-      <c r="O6" t="s">
-        <v>21</v>
-      </c>
-      <c r="P6" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="N7">
-        <v>46</v>
-      </c>
-      <c r="O7" t="s">
-        <v>23</v>
-      </c>
-      <c r="P7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="D8" s="7"/>
-      <c r="N8">
-        <v>47</v>
-      </c>
-      <c r="O8" t="s">
-        <v>25</v>
-      </c>
-      <c r="P8" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
     <mergeCell ref="A1:K1"/>
-    <mergeCell ref="O1:Q1"/>
   </mergeCells>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver" r:id="rId1"/>
+  <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
+  <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
+    <oddHeader/>
+    <oddFooter/>
+    <evenHeader/>
+    <evenFooter/>
+    <firstHeader/>
+    <firstFooter/>
+  </headerFooter>
+  <tableParts count="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xml:space="preserve" mc:Ignorable="x14ac">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
+      <selection activeCell="A6" sqref="A6:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="8.88671875" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" spans="1:4" customHeight="1" ht="21">
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="6"/>
+    </row>
+    <row r="2" spans="1:4" customHeight="1" ht="18">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="7">
+        <v>18</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="7">
+        <v>19</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="7">
+        <v>20</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="7">
+        <v>57</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
+  <mergeCells>
+    <mergeCell ref="B1:D1"/>
+  </mergeCells>
+  <printOptions gridLines="false" gridLinesSet="true"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="1" orientation="default" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
   <headerFooter differentOddEven="false" differentFirst="false" scaleWithDoc="true" alignWithMargins="true">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
kvalerio - validation cell functionality
</commit_message>
<xml_diff>
--- a/public/files/xlsx/Plantilla_Invitados.xlsx
+++ b/public/files/xlsx/Plantilla_Invitados.xlsx
@@ -647,7 +647,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A6" sqref="A6:D6"/>
@@ -655,14 +655,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="8.88671875" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" spans="1:4" customHeight="1" ht="21">
+    <row r="1" spans="1:6" customHeight="1" ht="21">
       <c r="B1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="C1" s="5"/>
       <c r="D1" s="6"/>
+      <c r="F1"/>
     </row>
-    <row r="2" spans="1:4" customHeight="1" ht="18">
+    <row r="2" spans="1:6" customHeight="1" ht="18">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -675,8 +676,9 @@
       <c r="D2" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="F2"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3" s="7">
         <v>18</v>
       </c>
@@ -689,8 +691,9 @@
       <c r="D3" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="F3"/>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4" s="7">
         <v>19</v>
       </c>
@@ -703,8 +706,9 @@
       <c r="D4" s="7" t="s">
         <v>20</v>
       </c>
+      <c r="F4"/>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:6">
       <c r="A5" s="7">
         <v>20</v>
       </c>
@@ -718,7 +722,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:6">
       <c r="A6" s="7">
         <v>57</v>
       </c>

</xml_diff>

<commit_message>
kvalerio - categories xlsx and subcategories
</commit_message>
<xml_diff>
--- a/public/files/xlsx/Plantilla_Invitados.xlsx
+++ b/public/files/xlsx/Plantilla_Invitados.xlsx
@@ -548,7 +548,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:Q24"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A3" sqref="A3:XFD6"/>
@@ -586,6 +586,7 @@
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
+      <c r="Q1"/>
     </row>
     <row r="2" spans="1:17" customHeight="1" ht="18">
       <c r="A2" s="2" t="s">
@@ -621,12 +622,95 @@
       <c r="K2" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="Q2"/>
+    </row>
+    <row r="3" spans="1:17" customHeight="1" ht="18">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="Q3"/>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="Q4"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="Q5"/>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="Q6"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="Q7"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="Q8"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="Q9"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="Q10"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="Q11"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="Q12"/>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="Q13"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="Q14"/>
+    </row>
+    <row r="15" spans="1:17">
+      <c r="Q15"/>
+    </row>
+    <row r="16" spans="1:17">
+      <c r="Q16"/>
+    </row>
+    <row r="17" spans="1:17">
+      <c r="Q17"/>
+    </row>
+    <row r="18" spans="1:17">
+      <c r="Q18"/>
+    </row>
+    <row r="19" spans="1:17">
+      <c r="Q19"/>
+    </row>
+    <row r="20" spans="1:17">
+      <c r="Q20"/>
+    </row>
+    <row r="21" spans="1:17">
+      <c r="Q21"/>
+    </row>
+    <row r="22" spans="1:17">
+      <c r="Q22"/>
+    </row>
+    <row r="23" spans="1:17">
+      <c r="Q23"/>
+    </row>
+    <row r="24" spans="1:17">
+      <c r="Q24"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
   <mergeCells>
     <mergeCell ref="A1:K1"/>
   </mergeCells>
+  <dataValidations count="1">
+    <dataValidation type="list" errorStyle="information" operator="between" allowBlank="0" showDropDown="0" showInputMessage="1" showErrorMessage="1" errorTitle="Error de entrada" error="No se ha seleccionado una categoria" promptTitle="Seleccione una categoria" prompt="Por favor seleccione una categoria para el invitado" sqref="F3">
+      <formula1>"Académico,Administrativo,Estudiante,Invitado"</formula1>
+    </dataValidation>
+  </dataValidations>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="1" orientation="portrait" scale="100" fitToHeight="1" fitToWidth="1" pageOrder="downThenOver"/>
@@ -691,7 +775,6 @@
       <c r="D3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F3"/>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="7">
@@ -706,7 +789,6 @@
       <c r="D4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F4"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="7">

</xml_diff>

<commit_message>
kvalerio - data validations
</commit_message>
<xml_diff>
--- a/public/files/xlsx/Plantilla_Invitados.xlsx
+++ b/public/files/xlsx/Plantilla_Invitados.xlsx
@@ -548,7 +548,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q24"/>
+  <dimension ref="A1:Q27"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A3" sqref="A3:XFD6"/>
@@ -700,6 +700,15 @@
     </row>
     <row r="24" spans="1:17">
       <c r="Q24"/>
+    </row>
+    <row r="25" spans="1:17">
+      <c r="Q25"/>
+    </row>
+    <row r="26" spans="1:17">
+      <c r="Q26"/>
+    </row>
+    <row r="27" spans="1:17">
+      <c r="Q27"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
kvalerio - person validation data
</commit_message>
<xml_diff>
--- a/public/files/xlsx/Plantilla_Invitados.xlsx
+++ b/public/files/xlsx/Plantilla_Invitados.xlsx
@@ -548,7 +548,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q27"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A3" sqref="A3:XFD6"/>
@@ -709,6 +709,15 @@
     </row>
     <row r="27" spans="1:17">
       <c r="Q27"/>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="Q28"/>
+    </row>
+    <row r="29" spans="1:17">
+      <c r="Q29"/>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="Q30"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>

</xml_diff>

<commit_message>
Addition and adjustments of reports
The report by person name is added and adjustments are made to the other reports in code
</commit_message>
<xml_diff>
--- a/public/files/xlsx/Plantilla_Invitados.xlsx
+++ b/public/files/xlsx/Plantilla_Invitados.xlsx
@@ -68,10 +68,10 @@
     <t>Estudiantes que reciben dinero y servicio de hospedaje</t>
   </si>
   <si>
-    <t>Emergencias</t>
-  </si>
-  <si>
-    <t>Equipos y más</t>
+    <t>Emergencias y rescate</t>
+  </si>
+  <si>
+    <t>Equipos y mas</t>
   </si>
   <si>
     <t>Mantenimientos</t>
@@ -80,10 +80,10 @@
     <t>Personal de limpieza de las areas de la universidads</t>
   </si>
   <si>
-    <t>Prueba</t>
-  </si>
-  <si>
-    <t>Desc Prueba</t>
+    <t>Ingles B2</t>
+  </si>
+  <si>
+    <t>Equipo de grammary</t>
   </si>
   <si>
     <t>Prueba2</t>
@@ -673,7 +673,7 @@
     </row>
     <row r="6" spans="1:17">
       <c r="N6">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="O6" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
kvalerio - last details upload xlsx functionality
</commit_message>
<xml_diff>
--- a/public/files/xlsx/Plantilla_Invitados.xlsx
+++ b/public/files/xlsx/Plantilla_Invitados.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
   <si>
     <t>Lista de personas</t>
   </si>
@@ -97,6 +97,15 @@
   </si>
   <si>
     <t>Allicia Vega</t>
+  </si>
+  <si>
+    <t>testSub</t>
+  </si>
+  <si>
+    <t>testdesS</t>
+  </si>
+  <si>
+    <t>testEnS</t>
   </si>
 </sst>
 </file>
@@ -548,7 +557,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q30"/>
+  <dimension ref="A1:Q189"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A3" sqref="A3:XFD6"/>
@@ -718,6 +727,483 @@
     </row>
     <row r="30" spans="1:17">
       <c r="Q30"/>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="Q31"/>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="Q32"/>
+    </row>
+    <row r="33" spans="1:17">
+      <c r="Q33"/>
+    </row>
+    <row r="34" spans="1:17">
+      <c r="Q34"/>
+    </row>
+    <row r="35" spans="1:17">
+      <c r="Q35"/>
+    </row>
+    <row r="36" spans="1:17">
+      <c r="Q36"/>
+    </row>
+    <row r="37" spans="1:17">
+      <c r="Q37"/>
+    </row>
+    <row r="38" spans="1:17">
+      <c r="Q38"/>
+    </row>
+    <row r="39" spans="1:17">
+      <c r="Q39"/>
+    </row>
+    <row r="40" spans="1:17">
+      <c r="Q40"/>
+    </row>
+    <row r="41" spans="1:17">
+      <c r="Q41"/>
+    </row>
+    <row r="42" spans="1:17">
+      <c r="Q42"/>
+    </row>
+    <row r="43" spans="1:17">
+      <c r="Q43"/>
+    </row>
+    <row r="44" spans="1:17">
+      <c r="Q44"/>
+    </row>
+    <row r="45" spans="1:17">
+      <c r="Q45"/>
+    </row>
+    <row r="46" spans="1:17">
+      <c r="Q46"/>
+    </row>
+    <row r="47" spans="1:17">
+      <c r="Q47"/>
+    </row>
+    <row r="48" spans="1:17">
+      <c r="Q48"/>
+    </row>
+    <row r="49" spans="1:17">
+      <c r="Q49"/>
+    </row>
+    <row r="50" spans="1:17">
+      <c r="Q50"/>
+    </row>
+    <row r="51" spans="1:17">
+      <c r="Q51"/>
+    </row>
+    <row r="52" spans="1:17">
+      <c r="Q52"/>
+    </row>
+    <row r="53" spans="1:17">
+      <c r="Q53"/>
+    </row>
+    <row r="54" spans="1:17">
+      <c r="Q54"/>
+    </row>
+    <row r="55" spans="1:17">
+      <c r="Q55"/>
+    </row>
+    <row r="56" spans="1:17">
+      <c r="Q56"/>
+    </row>
+    <row r="57" spans="1:17">
+      <c r="Q57"/>
+    </row>
+    <row r="58" spans="1:17">
+      <c r="Q58"/>
+    </row>
+    <row r="59" spans="1:17">
+      <c r="Q59"/>
+    </row>
+    <row r="60" spans="1:17">
+      <c r="Q60"/>
+    </row>
+    <row r="61" spans="1:17">
+      <c r="Q61"/>
+    </row>
+    <row r="62" spans="1:17">
+      <c r="Q62"/>
+    </row>
+    <row r="63" spans="1:17">
+      <c r="Q63"/>
+    </row>
+    <row r="64" spans="1:17">
+      <c r="Q64"/>
+    </row>
+    <row r="65" spans="1:17">
+      <c r="Q65"/>
+    </row>
+    <row r="66" spans="1:17">
+      <c r="Q66"/>
+    </row>
+    <row r="67" spans="1:17">
+      <c r="Q67"/>
+    </row>
+    <row r="68" spans="1:17">
+      <c r="Q68"/>
+    </row>
+    <row r="69" spans="1:17">
+      <c r="Q69"/>
+    </row>
+    <row r="70" spans="1:17">
+      <c r="Q70"/>
+    </row>
+    <row r="71" spans="1:17">
+      <c r="Q71"/>
+    </row>
+    <row r="72" spans="1:17">
+      <c r="Q72"/>
+    </row>
+    <row r="73" spans="1:17">
+      <c r="Q73"/>
+    </row>
+    <row r="74" spans="1:17">
+      <c r="Q74"/>
+    </row>
+    <row r="75" spans="1:17">
+      <c r="Q75"/>
+    </row>
+    <row r="76" spans="1:17">
+      <c r="Q76"/>
+    </row>
+    <row r="77" spans="1:17">
+      <c r="Q77"/>
+    </row>
+    <row r="78" spans="1:17">
+      <c r="Q78"/>
+    </row>
+    <row r="79" spans="1:17">
+      <c r="Q79"/>
+    </row>
+    <row r="80" spans="1:17">
+      <c r="Q80"/>
+    </row>
+    <row r="81" spans="1:17">
+      <c r="Q81"/>
+    </row>
+    <row r="82" spans="1:17">
+      <c r="Q82"/>
+    </row>
+    <row r="83" spans="1:17">
+      <c r="Q83"/>
+    </row>
+    <row r="84" spans="1:17">
+      <c r="Q84"/>
+    </row>
+    <row r="85" spans="1:17">
+      <c r="Q85"/>
+    </row>
+    <row r="86" spans="1:17">
+      <c r="Q86"/>
+    </row>
+    <row r="87" spans="1:17">
+      <c r="Q87"/>
+    </row>
+    <row r="88" spans="1:17">
+      <c r="Q88"/>
+    </row>
+    <row r="89" spans="1:17">
+      <c r="Q89"/>
+    </row>
+    <row r="90" spans="1:17">
+      <c r="Q90"/>
+    </row>
+    <row r="91" spans="1:17">
+      <c r="Q91"/>
+    </row>
+    <row r="92" spans="1:17">
+      <c r="Q92"/>
+    </row>
+    <row r="93" spans="1:17">
+      <c r="Q93"/>
+    </row>
+    <row r="94" spans="1:17">
+      <c r="Q94"/>
+    </row>
+    <row r="95" spans="1:17">
+      <c r="Q95"/>
+    </row>
+    <row r="96" spans="1:17">
+      <c r="Q96"/>
+    </row>
+    <row r="97" spans="1:17">
+      <c r="Q97"/>
+    </row>
+    <row r="98" spans="1:17">
+      <c r="Q98"/>
+    </row>
+    <row r="99" spans="1:17">
+      <c r="Q99"/>
+    </row>
+    <row r="100" spans="1:17">
+      <c r="Q100"/>
+    </row>
+    <row r="101" spans="1:17">
+      <c r="Q101"/>
+    </row>
+    <row r="102" spans="1:17">
+      <c r="Q102"/>
+    </row>
+    <row r="103" spans="1:17">
+      <c r="Q103"/>
+    </row>
+    <row r="104" spans="1:17">
+      <c r="Q104"/>
+    </row>
+    <row r="105" spans="1:17">
+      <c r="Q105"/>
+    </row>
+    <row r="106" spans="1:17">
+      <c r="Q106"/>
+    </row>
+    <row r="107" spans="1:17">
+      <c r="Q107"/>
+    </row>
+    <row r="108" spans="1:17">
+      <c r="Q108"/>
+    </row>
+    <row r="109" spans="1:17">
+      <c r="Q109"/>
+    </row>
+    <row r="110" spans="1:17">
+      <c r="Q110"/>
+    </row>
+    <row r="111" spans="1:17">
+      <c r="Q111"/>
+    </row>
+    <row r="112" spans="1:17">
+      <c r="Q112"/>
+    </row>
+    <row r="113" spans="1:17">
+      <c r="Q113"/>
+    </row>
+    <row r="114" spans="1:17">
+      <c r="Q114"/>
+    </row>
+    <row r="115" spans="1:17">
+      <c r="Q115"/>
+    </row>
+    <row r="116" spans="1:17">
+      <c r="Q116"/>
+    </row>
+    <row r="117" spans="1:17">
+      <c r="Q117"/>
+    </row>
+    <row r="118" spans="1:17">
+      <c r="Q118"/>
+    </row>
+    <row r="119" spans="1:17">
+      <c r="Q119"/>
+    </row>
+    <row r="120" spans="1:17">
+      <c r="Q120"/>
+    </row>
+    <row r="121" spans="1:17">
+      <c r="Q121"/>
+    </row>
+    <row r="122" spans="1:17">
+      <c r="Q122"/>
+    </row>
+    <row r="123" spans="1:17">
+      <c r="Q123"/>
+    </row>
+    <row r="124" spans="1:17">
+      <c r="Q124"/>
+    </row>
+    <row r="125" spans="1:17">
+      <c r="Q125"/>
+    </row>
+    <row r="126" spans="1:17">
+      <c r="Q126"/>
+    </row>
+    <row r="127" spans="1:17">
+      <c r="Q127"/>
+    </row>
+    <row r="128" spans="1:17">
+      <c r="Q128"/>
+    </row>
+    <row r="129" spans="1:17">
+      <c r="Q129"/>
+    </row>
+    <row r="130" spans="1:17">
+      <c r="Q130"/>
+    </row>
+    <row r="131" spans="1:17">
+      <c r="Q131"/>
+    </row>
+    <row r="132" spans="1:17">
+      <c r="Q132"/>
+    </row>
+    <row r="133" spans="1:17">
+      <c r="Q133"/>
+    </row>
+    <row r="134" spans="1:17">
+      <c r="Q134"/>
+    </row>
+    <row r="135" spans="1:17">
+      <c r="Q135"/>
+    </row>
+    <row r="136" spans="1:17">
+      <c r="Q136"/>
+    </row>
+    <row r="137" spans="1:17">
+      <c r="Q137"/>
+    </row>
+    <row r="138" spans="1:17">
+      <c r="Q138"/>
+    </row>
+    <row r="139" spans="1:17">
+      <c r="Q139"/>
+    </row>
+    <row r="140" spans="1:17">
+      <c r="Q140"/>
+    </row>
+    <row r="141" spans="1:17">
+      <c r="Q141"/>
+    </row>
+    <row r="142" spans="1:17">
+      <c r="Q142"/>
+    </row>
+    <row r="143" spans="1:17">
+      <c r="Q143"/>
+    </row>
+    <row r="144" spans="1:17">
+      <c r="Q144"/>
+    </row>
+    <row r="145" spans="1:17">
+      <c r="Q145"/>
+    </row>
+    <row r="146" spans="1:17">
+      <c r="Q146"/>
+    </row>
+    <row r="147" spans="1:17">
+      <c r="Q147"/>
+    </row>
+    <row r="148" spans="1:17">
+      <c r="Q148"/>
+    </row>
+    <row r="149" spans="1:17">
+      <c r="Q149"/>
+    </row>
+    <row r="150" spans="1:17">
+      <c r="Q150"/>
+    </row>
+    <row r="151" spans="1:17">
+      <c r="Q151"/>
+    </row>
+    <row r="152" spans="1:17">
+      <c r="Q152"/>
+    </row>
+    <row r="153" spans="1:17">
+      <c r="Q153"/>
+    </row>
+    <row r="154" spans="1:17">
+      <c r="Q154"/>
+    </row>
+    <row r="155" spans="1:17">
+      <c r="Q155"/>
+    </row>
+    <row r="156" spans="1:17">
+      <c r="Q156"/>
+    </row>
+    <row r="157" spans="1:17">
+      <c r="Q157"/>
+    </row>
+    <row r="158" spans="1:17">
+      <c r="Q158"/>
+    </row>
+    <row r="159" spans="1:17">
+      <c r="Q159"/>
+    </row>
+    <row r="160" spans="1:17">
+      <c r="Q160"/>
+    </row>
+    <row r="161" spans="1:17">
+      <c r="Q161"/>
+    </row>
+    <row r="162" spans="1:17">
+      <c r="Q162"/>
+    </row>
+    <row r="163" spans="1:17">
+      <c r="Q163"/>
+    </row>
+    <row r="164" spans="1:17">
+      <c r="Q164"/>
+    </row>
+    <row r="165" spans="1:17">
+      <c r="Q165"/>
+    </row>
+    <row r="166" spans="1:17">
+      <c r="Q166"/>
+    </row>
+    <row r="167" spans="1:17">
+      <c r="Q167"/>
+    </row>
+    <row r="168" spans="1:17">
+      <c r="Q168"/>
+    </row>
+    <row r="169" spans="1:17">
+      <c r="Q169"/>
+    </row>
+    <row r="170" spans="1:17">
+      <c r="Q170"/>
+    </row>
+    <row r="171" spans="1:17">
+      <c r="Q171"/>
+    </row>
+    <row r="172" spans="1:17">
+      <c r="Q172"/>
+    </row>
+    <row r="173" spans="1:17">
+      <c r="Q173"/>
+    </row>
+    <row r="174" spans="1:17">
+      <c r="Q174"/>
+    </row>
+    <row r="175" spans="1:17">
+      <c r="Q175"/>
+    </row>
+    <row r="176" spans="1:17">
+      <c r="Q176"/>
+    </row>
+    <row r="177" spans="1:17">
+      <c r="Q177"/>
+    </row>
+    <row r="178" spans="1:17">
+      <c r="Q178"/>
+    </row>
+    <row r="179" spans="1:17">
+      <c r="Q179"/>
+    </row>
+    <row r="180" spans="1:17">
+      <c r="Q180"/>
+    </row>
+    <row r="181" spans="1:17">
+      <c r="Q181"/>
+    </row>
+    <row r="182" spans="1:17">
+      <c r="Q182"/>
+    </row>
+    <row r="183" spans="1:17">
+      <c r="Q183"/>
+    </row>
+    <row r="184" spans="1:17">
+      <c r="Q184"/>
+    </row>
+    <row r="185" spans="1:17">
+      <c r="Q185"/>
+    </row>
+    <row r="186" spans="1:17">
+      <c r="Q186"/>
+    </row>
+    <row r="187" spans="1:17">
+      <c r="Q187"/>
+    </row>
+    <row r="188" spans="1:17">
+      <c r="Q188"/>
+    </row>
+    <row r="189" spans="1:17">
+      <c r="Q189"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -749,10 +1235,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A6" sqref="A6:D6"/>
+      <selection activeCell="A7" sqref="A7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="8.88671875" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -834,6 +1320,20 @@
       </c>
       <c r="D6" s="7" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="7">
+        <v>58</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[UPDATE] last details footer and navBar
</commit_message>
<xml_diff>
--- a/public/files/xlsx/Plantilla_Invitados.xlsx
+++ b/public/files/xlsx/Plantilla_Invitados.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="18">
   <si>
     <t>Lista de personas</t>
   </si>
@@ -63,49 +63,13 @@
     <t>Encargado</t>
   </si>
   <si>
-    <t>Becados</t>
-  </si>
-  <si>
-    <t>Estudiantes que reciben dinero y servicio de hospedaje</t>
-  </si>
-  <si>
-    <t>Mario Soto</t>
-  </si>
-  <si>
-    <t>Emergencias y rescate</t>
-  </si>
-  <si>
-    <t>Equipos y mas</t>
-  </si>
-  <si>
-    <t>Karla Mora</t>
-  </si>
-  <si>
-    <t>Mantenimientos</t>
-  </si>
-  <si>
-    <t>Personal de limpieza de las areas de la universidads</t>
-  </si>
-  <si>
-    <t>Juan Vindas</t>
-  </si>
-  <si>
-    <t>Ingles B2</t>
-  </si>
-  <si>
-    <t>Equipo de grammar</t>
-  </si>
-  <si>
-    <t>Allicia Vega</t>
-  </si>
-  <si>
-    <t>testSub</t>
-  </si>
-  <si>
-    <t>testdesS</t>
-  </si>
-  <si>
-    <t>testEnS</t>
+    <t>Becados LF</t>
+  </si>
+  <si>
+    <t>Becados LF Monto económico</t>
+  </si>
+  <si>
+    <t>Herminia Ávila</t>
   </si>
 </sst>
 </file>
@@ -557,7 +521,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:Q189"/>
+  <dimension ref="A1:Q219"/>
   <sheetViews>
     <sheetView tabSelected="0" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A3" sqref="A3:XFD6"/>
@@ -1204,6 +1168,96 @@
     </row>
     <row r="189" spans="1:17">
       <c r="Q189"/>
+    </row>
+    <row r="190" spans="1:17">
+      <c r="Q190"/>
+    </row>
+    <row r="191" spans="1:17">
+      <c r="Q191"/>
+    </row>
+    <row r="192" spans="1:17">
+      <c r="Q192"/>
+    </row>
+    <row r="193" spans="1:17">
+      <c r="Q193"/>
+    </row>
+    <row r="194" spans="1:17">
+      <c r="Q194"/>
+    </row>
+    <row r="195" spans="1:17">
+      <c r="Q195"/>
+    </row>
+    <row r="196" spans="1:17">
+      <c r="Q196"/>
+    </row>
+    <row r="197" spans="1:17">
+      <c r="Q197"/>
+    </row>
+    <row r="198" spans="1:17">
+      <c r="Q198"/>
+    </row>
+    <row r="199" spans="1:17">
+      <c r="Q199"/>
+    </row>
+    <row r="200" spans="1:17">
+      <c r="Q200"/>
+    </row>
+    <row r="201" spans="1:17">
+      <c r="Q201"/>
+    </row>
+    <row r="202" spans="1:17">
+      <c r="Q202"/>
+    </row>
+    <row r="203" spans="1:17">
+      <c r="Q203"/>
+    </row>
+    <row r="204" spans="1:17">
+      <c r="Q204"/>
+    </row>
+    <row r="205" spans="1:17">
+      <c r="Q205"/>
+    </row>
+    <row r="206" spans="1:17">
+      <c r="Q206"/>
+    </row>
+    <row r="207" spans="1:17">
+      <c r="Q207"/>
+    </row>
+    <row r="208" spans="1:17">
+      <c r="Q208"/>
+    </row>
+    <row r="209" spans="1:17">
+      <c r="Q209"/>
+    </row>
+    <row r="210" spans="1:17">
+      <c r="Q210"/>
+    </row>
+    <row r="211" spans="1:17">
+      <c r="Q211"/>
+    </row>
+    <row r="212" spans="1:17">
+      <c r="Q212"/>
+    </row>
+    <row r="213" spans="1:17">
+      <c r="Q213"/>
+    </row>
+    <row r="214" spans="1:17">
+      <c r="Q214"/>
+    </row>
+    <row r="215" spans="1:17">
+      <c r="Q215"/>
+    </row>
+    <row r="216" spans="1:17">
+      <c r="Q216"/>
+    </row>
+    <row r="217" spans="1:17">
+      <c r="Q217"/>
+    </row>
+    <row r="218" spans="1:17">
+      <c r="Q218"/>
+    </row>
+    <row r="219" spans="1:17">
+      <c r="Q219"/>
     </row>
   </sheetData>
   <sheetProtection sheet="false" objects="false" scenarios="false" formatCells="false" formatColumns="false" formatRows="false" insertColumns="false" insertRows="false" insertHyperlinks="false" deleteColumns="false" deleteRows="false" selectLockedCells="false" sort="false" autoFilter="false" pivotTables="false" selectUnlockedCells="false"/>
@@ -1235,10 +1289,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="A3" sqref="A3:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" defaultColWidth="8.88671875" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1268,7 +1322,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="7">
-        <v>18</v>
+        <v>59</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>15</v>
@@ -1278,62 +1332,6 @@
       </c>
       <c r="D3" s="7" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="7">
-        <v>19</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="7">
-        <v>20</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="7">
-        <v>57</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="7">
-        <v>58</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>